<commit_message>
[AV] Framework 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/[AV] Framework - 3237129936/[AV] Framework - 3237129936.xlsx
+++ b/Data/[AV] Framework - 3237129936/[AV] Framework - 3237129936.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\알티\[AV] Framework - 3237129936\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\[AV] Framework - 3237129936\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40309005-9FA0-4D63-BF65-88A37689C6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74979978-B5DB-4FB6-AB8D-1534C29F60A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="113">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -344,13 +344,30 @@
   </si>
   <si>
     <t>소비</t>
+  </si>
+  <si>
+    <t>ThingDef</t>
+  </si>
+  <si>
+    <t>Install {0_label} to become mechanitor</t>
+  </si>
+  <si>
+    <t>메카나이터가 되기 위해 {0_label} 설치</t>
+  </si>
+  <si>
+    <t>Mechlink.comps.CompUsableImplant_NoMechanitor.useLabel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ThingDef+Mechlink.comps.CompUsableImplant_NoMechanitor.useLabel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -368,6 +385,14 @@
       <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -390,9 +415,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -695,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1155,6 +1181,23 @@
         <v>107</v>
       </c>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>